<commit_message>
fix for wrong department data
</commit_message>
<xml_diff>
--- a/public/templates/employee_template.xlsx
+++ b/public/templates/employee_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RextLabo\ExcelExport\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RextLabo\ExcelExportLabo\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -114,9 +114,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -124,6 +121,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -409,57 +409,57 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="26.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>